<commit_message>
Add practice block | add diode test
</commit_message>
<xml_diff>
--- a/development/tests/passed_tests.xlsx
+++ b/development/tests/passed_tests.xlsx
@@ -3,19 +3,30 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AE434ED-EE23-4E51-BE34-FF66BC637FD1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A911703E-BF48-490E-ABB7-563C7D944F9B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="152">
   <si>
     <t>Conditions:</t>
   </si>
@@ -386,9 +397,6 @@
   </si>
   <si>
     <t>All words are imageable</t>
-  </si>
-  <si>
-    <t>Words don't repeat in stimuli list</t>
   </si>
   <si>
     <t>make sure both conditions exist:
@@ -466,6 +474,30 @@
   </si>
   <si>
     <t>make sure each trial set repeats the same amount of times.</t>
+  </si>
+  <si>
+    <t>return to start point (in getTraj.m)</t>
+  </si>
+  <si>
+    <t>Words don't repeat in stimuli list (word_freq_list)</t>
+  </si>
+  <si>
+    <t>Practice trials added to output file</t>
+  </si>
+  <si>
+    <t>appear before test trails.</t>
+  </si>
+  <si>
+    <t>are marked with practice = 1</t>
+  </si>
+  <si>
+    <t>all 40 exist.</t>
+  </si>
+  <si>
+    <t>Check 5 test trails appear after them correctly</t>
+  </si>
+  <si>
+    <t>practice and test trials aren't seperated by a header.</t>
   </si>
 </sst>
 </file>
@@ -972,11 +1004,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D111"/>
+  <dimension ref="A1:D117"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B109" sqref="B109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,7 +1023,7 @@
         <v>18</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>8</v>
@@ -1013,7 +1045,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -1023,7 +1055,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>115</v>
@@ -1045,7 +1077,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
@@ -1102,7 +1134,7 @@
     </row>
     <row r="12" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="10"/>
@@ -1113,14 +1145,14 @@
         <v>7</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="16"/>
@@ -1131,7 +1163,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -1151,7 +1183,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1210,114 +1242,111 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="18"/>
-      <c r="B27" s="16" t="s">
+      <c r="B27" s="29" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="18"/>
+      <c r="B28" s="16" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="18" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="B30" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="B29" s="16" t="s">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="28" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="28" t="s">
+      <c r="B31" s="29" t="s">
         <v>143</v>
       </c>
-      <c r="B30" s="29" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B32" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="7" t="s">
-        <v>10</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+      <c r="B33" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B34" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="7" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B35" s="22" t="s">
+      <c r="B36" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="23" t="s">
+      <c r="C36" s="20"/>
+      <c r="D36" s="20" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="23" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="B37" s="25" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="24" t="s">
-        <v>136</v>
+        <v>15</v>
+      </c>
+      <c r="B38" s="25" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
+      <c r="A39" s="24" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="17"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="18" t="s">
+      <c r="B40" s="17"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B40" s="16" t="s">
+      <c r="B41" s="16" t="s">
         <v>40</v>
-      </c>
-      <c r="D40" s="20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="18"/>
-      <c r="B41" s="16" t="s">
-        <v>41</v>
       </c>
       <c r="D41" s="20" t="s">
         <v>48</v>
@@ -1326,7 +1355,7 @@
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="18"/>
       <c r="B42" s="16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D42" s="20" t="s">
         <v>48</v>
@@ -1335,7 +1364,7 @@
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="18"/>
       <c r="B43" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D43" s="20" t="s">
         <v>48</v>
@@ -1344,7 +1373,7 @@
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="18"/>
       <c r="B44" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D44" s="20" t="s">
         <v>48</v>
@@ -1353,7 +1382,7 @@
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="18"/>
       <c r="B45" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D45" s="20" t="s">
         <v>48</v>
@@ -1362,7 +1391,7 @@
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="18"/>
       <c r="B46" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D46" s="20" t="s">
         <v>48</v>
@@ -1371,7 +1400,7 @@
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="18"/>
       <c r="B47" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D47" s="20" t="s">
         <v>48</v>
@@ -1380,7 +1409,7 @@
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="18"/>
       <c r="B48" s="16" t="s">
-        <v>134</v>
+        <v>47</v>
       </c>
       <c r="D48" s="20" t="s">
         <v>48</v>
@@ -1389,7 +1418,7 @@
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="18"/>
       <c r="B49" s="16" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D49" s="20" t="s">
         <v>48</v>
@@ -1398,7 +1427,7 @@
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="18"/>
       <c r="B50" s="16" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D50" s="20" t="s">
         <v>48</v>
@@ -1407,27 +1436,27 @@
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="18"/>
       <c r="B51" s="16" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D51" s="20" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="18" t="s">
-        <v>49</v>
-      </c>
+      <c r="A52" s="18"/>
       <c r="B52" s="16" t="s">
-        <v>50</v>
+        <v>132</v>
       </c>
       <c r="D52" s="20" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="18"/>
+      <c r="A53" s="18" t="s">
+        <v>49</v>
+      </c>
       <c r="B53" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D53" s="20" t="s">
         <v>48</v>
@@ -1436,7 +1465,7 @@
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="18"/>
       <c r="B54" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D54" s="20" t="s">
         <v>48</v>
@@ -1445,335 +1474,372 @@
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="18"/>
       <c r="B55" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D55" s="20" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="18" t="s">
-        <v>54</v>
-      </c>
+      <c r="A56" s="18"/>
       <c r="B56" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D56" s="20" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="18"/>
+      <c r="A57" s="18" t="s">
+        <v>54</v>
+      </c>
       <c r="B57" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D57" s="20" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="18"/>
+      <c r="B58" s="16" t="s">
+        <v>56</v>
+      </c>
       <c r="D58" s="20" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="8" t="s">
+      <c r="D59" s="20" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="B59" s="17"/>
-      <c r="C59" s="9"/>
-      <c r="D59" s="9"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B60" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="B60" s="17"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="B62" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C61" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B62" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="C62" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B63" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C63" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B64" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C63" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
+      <c r="C64" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B64" s="7" t="s">
+      <c r="B65" s="7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B65" s="7" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B66" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" s="7" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B67" s="7" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" s="7" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B68" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B68" s="7" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B69" s="7" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B69" s="7" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B70" s="7" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B70" s="7" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B71" s="7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B71" s="7" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B72" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B72" s="7" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B73" s="7" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B73" s="7" t="s">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B74" s="7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B74" s="7" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B75" s="7" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B75" s="7" t="s">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B76" s="7" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B76" s="7" t="s">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B77" s="7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B77" s="7" t="s">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B78" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B78" s="7" t="s">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B79" s="7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B79" s="7" t="s">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B80" s="7" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B80" s="7" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="82" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B82" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B87" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="88" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B88" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B90" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="91" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B91" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B92" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B93" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="94" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B94" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B95" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="96" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B96" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B97" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B98" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B99" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B100" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B101" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B102" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B103" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B104" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B105" s="7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="90" x14ac:dyDescent="0.25">
-      <c r="A105" s="4" t="s">
+    <row r="106" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A106" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="B105" s="6" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="B106" s="17"/>
-      <c r="C106" s="9"/>
-      <c r="D106" s="9"/>
+      <c r="B106" s="6" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B107" s="6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B108" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B109" s="6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B110" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B111" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B112" s="17"/>
+      <c r="C112" s="9"/>
+      <c r="D112" s="9"/>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A113" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="4" t="s">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="4" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="4" t="s">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B109" s="5" t="s">
+      <c r="B115" s="5" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="4" t="s">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A116" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="B110" s="5" t="s">
+      <c r="B116" s="5" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="4" t="s">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="B111" s="5" t="s">
+      <c r="B117" s="5" t="s">
         <v>113</v>
       </c>
     </row>

</xml_diff>